<commit_message>
Se actualizó la planilla de requerimientos
</commit_message>
<xml_diff>
--- a/Fase 2/Evidencias Proyecto/2.Planificación/Planilla_requerimientos_ FEATURING.xlsx
+++ b/Fase 2/Evidencias Proyecto/2.Planificación/Planilla_requerimientos_ FEATURING.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Featuring\Fase 2\Evidencias Proyecto\2.Planificación\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61B776D7-B349-4DE6-8AFF-7D5CFEDBA2C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4A26CB8-C0CE-4FD6-A8C6-F4788B38408D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -297,13 +297,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
+        <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -373,16 +373,16 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -604,7 +604,7 @@
   <dimension ref="A1:Z991"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="C2" sqref="C2:G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -680,7 +680,7 @@
       <c r="F2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="14" t="s">
         <v>59</v>
       </c>
     </row>
@@ -691,19 +691,19 @@
       <c r="B3" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="D3" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="15" t="s">
+      <c r="E3" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="15" t="s">
+      <c r="F3" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="G3" s="16" t="s">
+      <c r="G3" s="13" t="s">
         <v>61</v>
       </c>
     </row>
@@ -726,7 +726,7 @@
       <c r="F4" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="G4" s="14" t="s">
         <v>59</v>
       </c>
     </row>
@@ -749,7 +749,7 @@
       <c r="F5" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="G5" s="14" t="s">
         <v>59</v>
       </c>
     </row>
@@ -772,7 +772,7 @@
       <c r="F6" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="G6" s="7" t="s">
+      <c r="G6" s="14" t="s">
         <v>59</v>
       </c>
     </row>
@@ -795,7 +795,7 @@
       <c r="F7" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="G7" s="7" t="s">
+      <c r="G7" s="14" t="s">
         <v>59</v>
       </c>
     </row>
@@ -818,7 +818,7 @@
       <c r="F8" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="G8" s="7" t="s">
+      <c r="G8" s="14" t="s">
         <v>59</v>
       </c>
     </row>
@@ -841,7 +841,7 @@
       <c r="F9" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="G9" s="7" t="s">
+      <c r="G9" s="14" t="s">
         <v>59</v>
       </c>
     </row>
@@ -864,7 +864,7 @@
       <c r="F10" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G10" s="7" t="s">
+      <c r="G10" s="14" t="s">
         <v>59</v>
       </c>
     </row>
@@ -887,7 +887,7 @@
       <c r="F11" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="G11" s="7" t="s">
+      <c r="G11" s="14" t="s">
         <v>59</v>
       </c>
     </row>
@@ -910,7 +910,7 @@
       <c r="F12" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="G12" s="7" t="s">
+      <c r="G12" s="14" t="s">
         <v>59</v>
       </c>
     </row>
@@ -933,7 +933,7 @@
       <c r="F13" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="G13" s="13" t="s">
+      <c r="G13" s="15" t="s">
         <v>59</v>
       </c>
     </row>
@@ -956,7 +956,7 @@
       <c r="F14" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="G14" s="7" t="s">
+      <c r="G14" s="14" t="s">
         <v>59</v>
       </c>
     </row>
@@ -979,7 +979,7 @@
       <c r="F15" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="G15" s="12" t="s">
+      <c r="G15" s="16" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1002,7 +1002,7 @@
       <c r="F16" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="G16" s="7" t="s">
+      <c r="G16" s="14" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1025,7 +1025,7 @@
       <c r="F17" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="G17" s="14" t="s">
+      <c r="G17" s="16" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1048,7 +1048,7 @@
       <c r="F18" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="G18" s="14" t="s">
+      <c r="G18" s="16" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1071,7 +1071,7 @@
       <c r="F19" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="G19" s="12" t="s">
+      <c r="G19" s="16" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1094,7 +1094,7 @@
       <c r="F20" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="G20" s="12" t="s">
+      <c r="G20" s="16" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1117,7 +1117,7 @@
       <c r="F21" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="G21" s="12" t="s">
+      <c r="G21" s="16" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1140,7 +1140,7 @@
       <c r="F22" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="G22" s="12" t="s">
+      <c r="G22" s="16" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1163,7 +1163,7 @@
       <c r="F23" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="G23" s="12" t="s">
+      <c r="G23" s="16" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1186,7 +1186,7 @@
       <c r="F24" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="G24" s="14" t="s">
+      <c r="G24" s="16" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1203,7 +1203,7 @@
       <c r="F25" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="G25" s="12" t="s">
+      <c r="G25" s="16" t="s">
         <v>59</v>
       </c>
     </row>

</xml_diff>